<commit_message>
added topics for ds algo and behavioral
</commit_message>
<xml_diff>
--- a/PrepStatus.xlsx
+++ b/PrepStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jobs4\Intellij\PrepTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D46AA98-5D65-4B2A-8D83-62E4240152DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51821ECD-3973-4FC7-8885-AF161366FC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="1575" windowWidth="12225" windowHeight="11295" xr2:uid="{DFC65BCF-6B0B-4691-A374-E716F295FFA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFC65BCF-6B0B-4691-A374-E716F295FFA4}"/>
   </bookViews>
   <sheets>
     <sheet name="DS-Algo" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="156">
   <si>
     <t xml:space="preserve">LLD Topic </t>
   </si>
@@ -253,9 +253,6 @@
 Open/closed design with plugins or strategy pattern</t>
   </si>
   <si>
-    <t>Basic Design Exercises</t>
-  </si>
-  <si>
     <t>Interface vs Abstract Class
 Composition over Inheritance
 Favor immutability
@@ -270,14 +267,6 @@
 Interfaces and dependencies</t>
   </si>
   <si>
-    <t>Start with small ones:
-  Design a Stack using Queues
-  Design a Logger
-  Design a Tic Tac Toe
-  Design a Rate Limiter
-  Design an In-memory key-value store</t>
-  </si>
-  <si>
     <t>Model a system like Airflow or Step Functions
 DAGs, task execution, rollback, status tracking</t>
   </si>
@@ -417,6 +406,507 @@
   </si>
   <si>
     <t xml:space="preserve">Topic </t>
+  </si>
+  <si>
+    <t>Design a Stack using Queues</t>
+  </si>
+  <si>
+    <t>Design a Tic Tac Toe</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Easy Questions Solved</t>
+  </si>
+  <si>
+    <t>Medium Questions Solved</t>
+  </si>
+  <si>
+    <t>Hard Questions Solved</t>
+  </si>
+  <si>
+    <t>Use of TreeMap / TreeSet</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Design custom data structures </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   (e.g., LRU Cache, LFU Cache)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bit Manipulation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Single Number
+    Count Bits / Bitmask DP
+    XOR tricks</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tries &amp; Advanced DS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Implement Trie / Word Dictionary
+    Search Auto-complete
+    MapSum / Sum of Prefixes
+    Suffix Trie / Suffix Array (bonus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Heaps / Priority Queues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Kth Largest Element
+    Merge K Sorted Lists
+    Median in a Stream
+    Top K Frequent Elements
+📌 Always paired with HashMap in real interviews</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Greedy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Activity Selection
+    Merge Intervals
+    Minimum Platforms
+    Gas Station
+    Jump Game
+   Huffman Encoding (with Heap)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Graphs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    BFS / DFS
+    Topological Sort (Kahn’s Algo + DFS variant)
+    Cycle Detection (Directed &amp; Undirected)
+    Union Find / Disjoint Set
+    Shortest Path: Dijkstra / Bellman-Ford
+📌 Microsoft Favorites: Course Schedule, Number of Islands, Clone Graph</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dynamic Programming (DP)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   1D DP: Fibonacci, House Robber, Climbing Stairs
+   2D DP: Knapsack, Unique Paths, Edit Distance
+   DP with Memoization vs Tabulation
+   DP on Strings: LCS, Longest Palindromic Substring
+   DP on Trees / DP on Grids
+📌 Microsoft loves: Optimization of recursive problems with DP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Recursion &amp; Backtracking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   N-Queens / Sudoku Solver
+   Generate Parentheses
+   Permutations / Subsets / Combinations
+   Word Search
+📌 Tested: Design interview + optimization required</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Binary Search &amp; Search Variants</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Classic Binary Search
+    Find element in rotated sorted array
+    Binary Search on Answer (e.g., min days to ship packages)
+    Matrix Search (Sorted Matrix)
+📌 Hot for Seniors: When to use binary search on value range instead of array</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trees &amp; Binary Trees</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Inorder / Preorder / Postorder (Recursive + Iterative)
+    Level Order / Zigzag / Vertical Order
+    Lowest Common Ancestor (LCA)
+    Validate BST
+    Diameter of Tree
+    Symmetric Tree / Mirror Tree
+📌 Important: Binary Tree Path Sum variants</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stacks &amp; Queues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Monotonic Stack (Next Greater Element, Stock Span)
+    Min Stack / Implement Stack using Queue
+    BFS using Queue
+    Sliding Window Maximum (Deque)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linked List</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Reverse Linked List (iterative + recursive)
+    Detect Cycle (Floyd’s algorithm)
+    Merge Two Sorted Lists
+    Intersection Point of Two Lists
+    Reorder List, Rotate List
+📌 Tricky Variant: Flatten multilevel doubly linked list</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hashing / HashMap / HashSet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Frequency counting
+    Two Sum / Four Sum / Subarray with 0 sum
+    Group Anagrams / Longest Consecutive Sequence
+    HashMap + Sliding Window
+📌 Must Know: Custom key hashing (Map&lt;Pair, Integer&gt;)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Arrays &amp; Strings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+     Sliding Window (max sum, min subarray, longest substring without repeat)
+    Two Pointers (merge sorted arrays, partitioning, reverse in-place)
+    Prefix Sum &amp; Difference Arrays
+    Kadane’s Algorithm (Maximum Subarray)
+📌 Patterns: Dutch National Flag, Subarray sum = k, Binary search on answer</t>
+    </r>
+  </si>
+  <si>
+    <t>Basic Intro/Info/Theory</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer1 </t>
+  </si>
+  <si>
+    <t>Answer2</t>
+  </si>
+  <si>
+    <t>Answer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teamwork &amp; Collaboration</t>
+  </si>
+  <si>
+    <t>Tell me about a time you had a conflict with a team member. How did you resolve it?</t>
+  </si>
+  <si>
+    <t>Describe a time when you helped a teammate grow or succeed.</t>
+  </si>
+  <si>
+    <t>How do you handle working with cross-functional teams (QA, PM, Ops)?</t>
+  </si>
+  <si>
+    <t>Ownership &amp; Leadership</t>
+  </si>
+  <si>
+    <t>Tell me about a time you took ownership of a problem end-to-end.</t>
+  </si>
+  <si>
+    <t>Have you ever challenged a decision or proposed a better solution?</t>
+  </si>
+  <si>
+    <t>How do you mentor or coach junior developers?</t>
+  </si>
+  <si>
+    <t>Problem Solving &amp; Impact</t>
+  </si>
+  <si>
+    <t>Describe a complex technical problem you solved and how you approached it.</t>
+  </si>
+  <si>
+    <t>Have you ever worked under tight deadlines? What did you do?</t>
+  </si>
+  <si>
+    <t>Tell me about a system you improved or optimized. What was the impact?</t>
+  </si>
+  <si>
+    <t>Customer Focus</t>
+  </si>
+  <si>
+    <t>Tell me about a time you advocated for customer needs.</t>
+  </si>
+  <si>
+    <t>How do you ensure that your solution aligns with the user’s requirements?</t>
+  </si>
+  <si>
+    <t>Dealing with Ambiguity</t>
+  </si>
+  <si>
+    <t>Describe a situation where the requirements were unclear. What did you do?</t>
+  </si>
+  <si>
+    <t>Tell me about a time you had to make a decision without having all the information.</t>
+  </si>
+  <si>
+    <t>Failures &amp; Learning</t>
+  </si>
+  <si>
+    <t>Tell me about a mistake you made. What did you learn from it?</t>
+  </si>
+  <si>
+    <t>Have you ever built something that failed or didn’t meet expectations?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Microsoft Culture Fit</t>
+  </si>
+  <si>
+    <t>Why Microsoft?</t>
+  </si>
+  <si>
+    <t>What do you value in a team?</t>
+  </si>
+  <si>
+    <t>How do you stay current with technology?</t>
   </si>
 </sst>
 </file>
@@ -786,24 +1276,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3907C2C0-61B2-45D4-8E7F-6CE8F41FB6FB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="71.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B1DFE-1CFF-42B4-A26F-49FC90DF550F}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +1455,7 @@
         <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -869,7 +1463,7 @@
         <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -888,24 +1482,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="4"/>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,138 +1547,143 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>61</v>
+      <c r="B42" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1099,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544801E1-AF3C-4208-9B9E-60493BA108FD}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,220 +1711,220 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1337,14 +1934,160 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EB5C8-EFFB-40D7-80FA-825D28457C76}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="93.85546875" customWidth="1"/>
+    <col min="2" max="2" width="108.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>